<commit_message>
add excel date supported and refactor api
</commit_message>
<xml_diff>
--- a/src/test/resources/me/excel/tools/importer/test.xlsx
+++ b/src/test/resources/me/excel/tools/importer/test.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanwen/workspace/idea-projects-os/java-excel-tools/src/test/resources/me/excel/tools/importer/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="19710" windowHeight="8580"/>
+    <workbookView xWindow="800" yWindow="460" windowWidth="24800" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>学号</t>
   </si>
@@ -47,12 +60,6 @@
   </si>
   <si>
     <t>std1</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>2015-09-01</t>
   </si>
   <si>
     <t>2222</t>
@@ -64,14 +71,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="方正书宋_GBK"/>
@@ -95,39 +99,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="千位分隔" xfId="2" builtinId="3"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -426,6 +423,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -458,20 +456,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="14.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -499,7 +496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -513,36 +510,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
+      <c r="C5" s="2">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42249</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>